<commit_message>
Finalized JUnit tests and text descriptions.
</commit_message>
<xml_diff>
--- a/ClueFiles/map.xlsx
+++ b/ClueFiles/map.xlsx
@@ -55,9 +55,6 @@
     <t>E</t>
   </si>
   <si>
-    <t>ER</t>
-  </si>
-  <si>
     <t>I</t>
   </si>
   <si>
@@ -78,12 +75,15 @@
   <si>
     <t>ED</t>
   </si>
+  <si>
+    <t>EU</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -102,6 +102,17 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -124,7 +135,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -132,6 +143,8 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -619,7 +632,7 @@
   <dimension ref="A1:V23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1277,8 +1290,8 @@
       <c r="M10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N10" s="1" t="s">
-        <v>12</v>
+      <c r="N10" s="6" t="s">
+        <v>20</v>
       </c>
       <c r="O10" s="1" t="s">
         <v>12</v>
@@ -1411,26 +1424,26 @@
       <c r="N12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O12" s="3" t="s">
+      <c r="O12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="P12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q12" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R12" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="S12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U12" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1438,64 +1451,64 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="P13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="R13" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="I13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="M13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="P13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="R13" s="3" t="s">
-        <v>16</v>
-      </c>
       <c r="S13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U13" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="14" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1503,16 +1516,16 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>1</v>
@@ -1551,16 +1564,16 @@
         <v>1</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="15" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1568,16 +1581,16 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>1</v>
@@ -1616,16 +1629,16 @@
         <v>1</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1633,16 +1646,16 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>1</v>
@@ -1681,16 +1694,16 @@
         <v>1</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U16" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1698,16 +1711,16 @@
         <v>14</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
         <v>1</v>
@@ -1746,16 +1759,16 @@
         <v>1</v>
       </c>
       <c r="R17" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1763,16 +1776,16 @@
         <v>15</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>1</v>
@@ -1811,16 +1824,16 @@
         <v>1</v>
       </c>
       <c r="R18" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="S18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1828,16 +1841,16 @@
         <v>16</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>1</v>
@@ -1876,16 +1889,16 @@
         <v>1</v>
       </c>
       <c r="R19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1893,16 +1906,16 @@
         <v>17</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>1</v>
@@ -1926,7 +1939,7 @@
         <v>12</v>
       </c>
       <c r="M20" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="N20" s="1" t="s">
         <v>12</v>
@@ -1941,16 +1954,16 @@
         <v>1</v>
       </c>
       <c r="R20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="S20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="U20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2213,5 +2226,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Finished adj and target tests
</commit_message>
<xml_diff>
--- a/ClueFiles/map.xlsx
+++ b/ClueFiles/map.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="28">
   <si>
     <t>X</t>
   </si>
@@ -80,6 +80,24 @@
   </si>
   <si>
     <t>E ^</t>
+  </si>
+  <si>
+    <t>White: Door Direction Tests from OurTests</t>
+  </si>
+  <si>
+    <t>Orange: Adj Lists inside room</t>
+  </si>
+  <si>
+    <t>Purple: Adj Lists room exits</t>
+  </si>
+  <si>
+    <t>Olive Green: Adj Lists besides room entrances</t>
+  </si>
+  <si>
+    <t>Blue: Walkway tests</t>
+  </si>
+  <si>
+    <t>Grey: Target tests</t>
   </si>
 </sst>
 </file>
@@ -175,7 +193,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -185,7 +203,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -193,11 +210,741 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="65">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF980000"/>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF980000"/>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9900FF"/>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4A86E8"/>
+          <bgColor rgb="FF4A86E8"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8E7CC3"/>
+          <bgColor rgb="FF8E7CC3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF980000"/>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF980000"/>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9900FF"/>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4A86E8"/>
+          <bgColor rgb="FF4A86E8"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8E7CC3"/>
+          <bgColor rgb="FF8E7CC3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF980000"/>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF980000"/>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9900FF"/>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4A86E8"/>
+          <bgColor rgb="FF4A86E8"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8E7CC3"/>
+          <bgColor rgb="FF8E7CC3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF980000"/>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF980000"/>
+          <bgColor rgb="FF980000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF00FF"/>
+          <bgColor rgb="FFFF00FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF9900FF"/>
+          <bgColor rgb="FF9900FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF0000FF"/>
+          <bgColor rgb="FF0000FF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF4A86E8"/>
+          <bgColor rgb="FF4A86E8"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FFFF"/>
+          <bgColor rgb="FF00FFFF"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF00FF00"/>
+          <bgColor rgb="FF00FF00"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF8E7CC3"/>
+          <bgColor rgb="FF8E7CC3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF9900"/>
+          <bgColor rgb="FFFF9900"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFB7E1CD"/>
+          <bgColor rgb="FFB7E1CD"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4C7C3"/>
+          <bgColor rgb="FFF4C7C3"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -680,10 +1427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V23"/>
+  <dimension ref="A1:V30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -715,7 +1462,7 @@
       <c r="A1" s="1">
         <v>0</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
@@ -748,7 +1495,7 @@
       <c r="L1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="14" t="s">
+      <c r="M1" s="13" t="s">
         <v>1</v>
       </c>
       <c r="N1" s="1" t="s">
@@ -760,7 +1507,7 @@
       <c r="P1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="12" t="s">
+      <c r="Q1" s="11" t="s">
         <v>1</v>
       </c>
       <c r="R1" s="1" t="s">
@@ -925,7 +1672,7 @@
       <c r="E4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -940,7 +1687,7 @@
       <c r="J4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="K4" s="12" t="s">
+      <c r="K4" s="11" t="s">
         <v>1</v>
       </c>
       <c r="L4" s="1" t="s">
@@ -1134,10 +1881,10 @@
       <c r="I7" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="J7" s="12" t="s">
-        <v>1</v>
-      </c>
-      <c r="K7" s="1" t="s">
+      <c r="J7" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K7" s="12" t="s">
         <v>1</v>
       </c>
       <c r="L7" s="1" t="s">
@@ -1152,7 +1899,7 @@
       <c r="O7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="P7" s="13" t="s">
+      <c r="P7" s="12" t="s">
         <v>1</v>
       </c>
       <c r="Q7" s="1" t="s">
@@ -1223,13 +1970,13 @@
       <c r="Q8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R8" s="9" t="s">
+      <c r="R8" s="8" t="s">
         <v>8</v>
       </c>
       <c r="S8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="T8" s="8" t="s">
+      <c r="T8" s="7" t="s">
         <v>6</v>
       </c>
       <c r="U8" s="1" t="s">
@@ -1252,7 +1999,7 @@
       <c r="E9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="11" t="s">
+      <c r="F9" s="10" t="s">
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
@@ -1264,7 +2011,7 @@
       <c r="I9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="8" t="s">
+      <c r="J9" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K9" s="1" t="s">
@@ -1276,7 +2023,7 @@
       <c r="M9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="N9" s="11" t="s">
+      <c r="N9" s="10" t="s">
         <v>1</v>
       </c>
       <c r="O9" s="1" t="s">
@@ -1407,7 +2154,7 @@
       <c r="M11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N11" s="10" t="s">
+      <c r="N11" s="9" t="s">
         <v>21</v>
       </c>
       <c r="O11" s="1" t="s">
@@ -1519,7 +2266,7 @@
       <c r="G13" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="H13" s="8" t="s">
+      <c r="H13" s="7" t="s">
         <v>10</v>
       </c>
       <c r="I13" s="1" t="s">
@@ -1705,7 +2452,7 @@
       <c r="D16" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="8" t="s">
         <v>17</v>
       </c>
       <c r="F16" s="1" t="s">
@@ -1770,7 +2517,7 @@
       <c r="D17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E17" s="7" t="s">
         <v>14</v>
       </c>
       <c r="F17" s="1" t="s">
@@ -1806,7 +2553,7 @@
       <c r="P17" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="Q17" s="10" t="s">
         <v>1</v>
       </c>
       <c r="R17" s="4" t="s">
@@ -1874,7 +2621,7 @@
       <c r="Q18" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R18" s="7" t="s">
+      <c r="R18" s="14" t="s">
         <v>18</v>
       </c>
       <c r="S18" s="1" t="s">
@@ -1980,7 +2727,7 @@
       <c r="I20" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="J20" s="8" t="s">
+      <c r="J20" s="7" t="s">
         <v>10</v>
       </c>
       <c r="K20" s="1" t="s">
@@ -1989,7 +2736,7 @@
       <c r="L20" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M20" s="9" t="s">
+      <c r="M20" s="8" t="s">
         <v>19</v>
       </c>
       <c r="N20" s="1" t="s">
@@ -2004,7 +2751,7 @@
       <c r="Q20" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="R20" s="8" t="s">
+      <c r="R20" s="7" t="s">
         <v>16</v>
       </c>
       <c r="S20" s="1" t="s">
@@ -2013,7 +2760,7 @@
       <c r="T20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U20" s="8" t="s">
+      <c r="U20" s="7" t="s">
         <v>16</v>
       </c>
     </row>
@@ -2054,7 +2801,7 @@
       <c r="L21" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M21" s="11" t="s">
+      <c r="M21" s="10" t="s">
         <v>1</v>
       </c>
       <c r="N21" s="1" t="s">
@@ -2098,7 +2845,7 @@
       <c r="E22" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="F22" s="1" t="s">
+      <c r="F22" s="12" t="s">
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
@@ -2107,7 +2854,7 @@
       <c r="H22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="I22" s="12" t="s">
+      <c r="I22" s="11" t="s">
         <v>1</v>
       </c>
       <c r="J22" s="1" t="s">
@@ -2131,7 +2878,7 @@
       <c r="P22" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="Q22" s="1" t="s">
+      <c r="Q22" s="12" t="s">
         <v>1</v>
       </c>
       <c r="R22" s="1" t="s">
@@ -2210,69 +2957,99 @@
       </c>
       <c r="V23" s="1"/>
     </row>
+    <row r="25" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B26" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B27" s="15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B28" s="15" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B29" s="15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="30" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B30" s="15" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="X">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="64" priority="1" operator="containsText" text="X">
       <formula>NOT(ISERROR(SEARCH(("X"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="W">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="63" priority="2" operator="containsText" text="W">
       <formula>NOT(ISERROR(SEARCH(("W"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="A">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="62" priority="3" operator="containsText" text="A">
       <formula>NOT(ISERROR(SEARCH(("A"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="B">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="61" priority="4" operator="containsText" text="B">
       <formula>NOT(ISERROR(SEARCH(("B"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="C">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="60" priority="5" operator="containsText" text="C">
       <formula>NOT(ISERROR(SEARCH(("C"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="E">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="59" priority="6" operator="containsText" text="E">
       <formula>NOT(ISERROR(SEARCH(("E"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="F">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="58" priority="7" operator="containsText" text="F">
       <formula>NOT(ISERROR(SEARCH(("F"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="G">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="57" priority="8" operator="containsText" text="G">
       <formula>NOT(ISERROR(SEARCH(("G"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="4" priority="9" operator="containsText" text="H">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="56" priority="9" operator="containsText" text="H">
       <formula>NOT(ISERROR(SEARCH(("H"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="3" priority="10" operator="containsText" text="I">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="55" priority="10" operator="containsText" text="I">
       <formula>NOT(ISERROR(SEARCH(("I"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:U18 C1:E1 G1:L1 B22:H22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:U22 L4:U4 K7:M7 R1:U1 G4 Q7:U7 N1:P1">
-    <cfRule type="containsText" dxfId="2" priority="11" operator="containsText" text="J">
+  <conditionalFormatting sqref="B2:U3 B8:Q8 B7:I7 O7 B12:U15 B5:U6 B4:E4 I4:J4 B9:D9 G9:I9 B19:U19 B18:H18 J18:Q18 C1:E1 G1:L1 B22:E22 B20:I20 N20:T20 B16:D17 U8 F16:U16 K9:M9 K20:L20 S8 B10:M11 B21:L21 N21:U21 O9:U11 F17:P17 R17:U17 J22:P22 L4:U4 L7:M7 R1:U1 G4 Q7:U7 N1:P1 G22:H22 R22:U22 S18:U18">
+    <cfRule type="containsText" dxfId="54" priority="11" operator="containsText" text="J">
       <formula>NOT(ISERROR(SEARCH(("J"),(B1))))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G19">
-    <cfRule type="endsWith" dxfId="1" priority="12" operator="endsWith" text="-">
+    <cfRule type="endsWith" dxfId="53" priority="12" operator="endsWith" text="-">
       <formula>RIGHT((G19),LEN("-"))=("-")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W16">
-    <cfRule type="containsText" dxfId="0" priority="13" operator="containsText" text="-">
+    <cfRule type="containsText" dxfId="52" priority="13" operator="containsText" text="-">
       <formula>NOT(ISERROR(SEARCH(("-"),(W16))))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>